<commit_message>
Gantt Chart Update - Week 9
</commit_message>
<xml_diff>
--- a/Gantt-diagram(projektplan).xlsx
+++ b/Gantt-diagram(projektplan).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khali\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathi\Documents\Hardware-identification-and-QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3684229-1020-41F6-9362-BB7984A654E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254B5C8E-D8B6-40CB-9DFE-7A8CD623C21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1335" yWindow="4065" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplanlægger" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <r>
       <rPr>
@@ -231,19 +231,16 @@
     <t>Gantt Project Planner - Weeks, Overview (Quality Assurance, Otovo group)</t>
   </si>
   <si>
-    <t>1. implementation of retrained OCR &amp; STR models</t>
-  </si>
-  <si>
     <t>Research influence of resolution on accuracy</t>
   </si>
   <si>
-    <t>Michael</t>
-  </si>
-  <si>
     <t>Mid-way report</t>
   </si>
   <si>
     <t>Give peer review to other projects</t>
+  </si>
+  <si>
+    <t>1. implementation of retrained OCR &amp; STR models using HPC</t>
   </si>
 </sst>
 </file>
@@ -413,7 +410,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -816,77 +812,77 @@
     <xf numFmtId="1" fontId="12" fillId="10" borderId="1" xfId="13" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="12" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="12" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1426,26 +1422,26 @@
   </sheetPr>
   <dimension ref="A1:EI66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="25" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.58203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.25" style="2" customWidth="1"/>
+    <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="3" customWidth="1"/>
-    <col min="8" max="8" width="3.1640625" style="1" customWidth="1"/>
-    <col min="9" max="27" width="3.58203125" style="1" customWidth="1"/>
-    <col min="28" max="77" width="3.58203125" customWidth="1"/>
-    <col min="79" max="97" width="2.9140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.125" style="1" customWidth="1"/>
+    <col min="9" max="27" width="3.625" style="1" customWidth="1"/>
+    <col min="28" max="77" width="3.625" customWidth="1"/>
+    <col min="79" max="97" width="2.875" bestFit="1" customWidth="1"/>
     <col min="98" max="118" width="1.25" customWidth="1"/>
-    <col min="119" max="125" width="4.08203125" bestFit="1" customWidth="1"/>
+    <col min="119" max="125" width="4.125" bestFit="1" customWidth="1"/>
     <col min="126" max="146" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:139" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
+    <row r="1" spans="1:139" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="7" t="s">
         <v>42</v>
       </c>
@@ -1455,196 +1451,196 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:139" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+    <row r="2" spans="1:139" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="43"/>
       <c r="H2" s="44"/>
       <c r="J2" s="8"/>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="61"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="60"/>
       <c r="P2" s="9"/>
-      <c r="Q2" s="59" t="s">
+      <c r="Q2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="61"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="60"/>
       <c r="U2" s="10"/>
-      <c r="V2" s="62" t="s">
+      <c r="V2" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="63"/>
-      <c r="X2" s="63"/>
-      <c r="Y2" s="64"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="63"/>
       <c r="Z2" s="11"/>
-      <c r="AA2" s="65" t="s">
+      <c r="AA2" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="67"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="66"/>
       <c r="AH2" s="12"/>
-      <c r="AI2" s="62" t="s">
+      <c r="AI2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="AJ2" s="63"/>
-      <c r="AK2" s="63"/>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-    </row>
-    <row r="3" spans="1:139" s="5" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
+      <c r="AJ2" s="62"/>
+      <c r="AK2" s="62"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+    </row>
+    <row r="3" spans="1:139" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="45" t="s">
+      <c r="H3" s="49"/>
+      <c r="I3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="47" t="s">
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="45" t="s">
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="47" t="s">
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="AC3" s="47"/>
-      <c r="AD3" s="47"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="47"/>
-      <c r="AH3" s="47"/>
-      <c r="AI3" s="45" t="s">
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="45"/>
-      <c r="AL3" s="45"/>
-      <c r="AM3" s="45"/>
-      <c r="AN3" s="45"/>
-      <c r="AO3" s="45"/>
-      <c r="AP3" s="47" t="s">
+      <c r="AJ3" s="67"/>
+      <c r="AK3" s="67"/>
+      <c r="AL3" s="67"/>
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="47"/>
-      <c r="AR3" s="47"/>
-      <c r="AS3" s="47"/>
-      <c r="AT3" s="47"/>
-      <c r="AU3" s="47"/>
-      <c r="AV3" s="47"/>
-      <c r="AW3" s="45" t="s">
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+      <c r="AV3" s="68"/>
+      <c r="AW3" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="AX3" s="45"/>
-      <c r="AY3" s="45"/>
-      <c r="AZ3" s="45"/>
-      <c r="BA3" s="45"/>
-      <c r="BB3" s="45"/>
-      <c r="BC3" s="45"/>
-      <c r="BD3" s="47" t="s">
+      <c r="AX3" s="67"/>
+      <c r="AY3" s="67"/>
+      <c r="AZ3" s="67"/>
+      <c r="BA3" s="67"/>
+      <c r="BB3" s="67"/>
+      <c r="BC3" s="67"/>
+      <c r="BD3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="BE3" s="47"/>
-      <c r="BF3" s="47"/>
-      <c r="BG3" s="47"/>
-      <c r="BH3" s="47"/>
-      <c r="BI3" s="47"/>
-      <c r="BJ3" s="47"/>
-      <c r="BK3" s="45" t="s">
+      <c r="BE3" s="68"/>
+      <c r="BF3" s="68"/>
+      <c r="BG3" s="68"/>
+      <c r="BH3" s="68"/>
+      <c r="BI3" s="68"/>
+      <c r="BJ3" s="68"/>
+      <c r="BK3" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="BL3" s="45"/>
-      <c r="BM3" s="45"/>
-      <c r="BN3" s="45"/>
-      <c r="BO3" s="45"/>
-      <c r="BP3" s="45"/>
-      <c r="BQ3" s="45"/>
-      <c r="BR3" s="47" t="s">
+      <c r="BL3" s="67"/>
+      <c r="BM3" s="67"/>
+      <c r="BN3" s="67"/>
+      <c r="BO3" s="67"/>
+      <c r="BP3" s="67"/>
+      <c r="BQ3" s="67"/>
+      <c r="BR3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="BS3" s="47"/>
-      <c r="BT3" s="47"/>
-      <c r="BU3" s="47"/>
-      <c r="BV3" s="47"/>
-      <c r="BW3" s="47"/>
-      <c r="BX3" s="47"/>
-      <c r="BY3" s="45" t="s">
+      <c r="BS3" s="68"/>
+      <c r="BT3" s="68"/>
+      <c r="BU3" s="68"/>
+      <c r="BV3" s="68"/>
+      <c r="BW3" s="68"/>
+      <c r="BX3" s="68"/>
+      <c r="BY3" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="BZ3" s="45"/>
-      <c r="CA3" s="45"/>
-      <c r="CB3" s="45"/>
-      <c r="CC3" s="45"/>
-      <c r="CD3" s="45"/>
-      <c r="CE3" s="45"/>
-      <c r="CF3" s="47" t="s">
+      <c r="BZ3" s="67"/>
+      <c r="CA3" s="67"/>
+      <c r="CB3" s="67"/>
+      <c r="CC3" s="67"/>
+      <c r="CD3" s="67"/>
+      <c r="CE3" s="67"/>
+      <c r="CF3" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="CG3" s="47"/>
-      <c r="CH3" s="47"/>
-      <c r="CI3" s="47"/>
-      <c r="CJ3" s="47"/>
-      <c r="CK3" s="47"/>
-      <c r="CL3" s="47"/>
-      <c r="CM3" s="45" t="s">
+      <c r="CG3" s="68"/>
+      <c r="CH3" s="68"/>
+      <c r="CI3" s="68"/>
+      <c r="CJ3" s="68"/>
+      <c r="CK3" s="68"/>
+      <c r="CL3" s="68"/>
+      <c r="CM3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="CN3" s="45"/>
-      <c r="CO3" s="45"/>
-      <c r="CP3" s="45"/>
-      <c r="CQ3" s="45"/>
-      <c r="CR3" s="45"/>
-      <c r="CS3" s="45"/>
+      <c r="CN3" s="67"/>
+      <c r="CO3" s="67"/>
+      <c r="CP3" s="67"/>
+      <c r="CQ3" s="67"/>
+      <c r="CR3" s="67"/>
+      <c r="CS3" s="67"/>
       <c r="CT3" s="46"/>
       <c r="CU3" s="46"/>
       <c r="CV3" s="46"/>
@@ -1668,39 +1664,39 @@
       <c r="DL3" s="46"/>
       <c r="DM3" s="46"/>
       <c r="DN3" s="46"/>
-      <c r="DO3" s="45" t="s">
+      <c r="DO3" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="DP3" s="45"/>
-      <c r="DQ3" s="45"/>
-      <c r="DR3" s="45"/>
-      <c r="DS3" s="45"/>
-      <c r="DT3" s="45"/>
-      <c r="DU3" s="45"/>
-      <c r="DV3" s="45"/>
-      <c r="DW3" s="45"/>
-      <c r="DX3" s="45"/>
-      <c r="DY3" s="45"/>
-      <c r="DZ3" s="45"/>
-      <c r="EA3" s="45"/>
-      <c r="EB3" s="45"/>
-      <c r="EC3" s="45"/>
-      <c r="ED3" s="45"/>
-      <c r="EE3" s="45"/>
-      <c r="EF3" s="45"/>
-      <c r="EG3" s="45"/>
-      <c r="EH3" s="45"/>
-      <c r="EI3" s="45"/>
-    </row>
-    <row r="4" spans="1:139" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="51"/>
+      <c r="DP3" s="67"/>
+      <c r="DQ3" s="67"/>
+      <c r="DR3" s="67"/>
+      <c r="DS3" s="67"/>
+      <c r="DT3" s="67"/>
+      <c r="DU3" s="67"/>
+      <c r="DV3" s="67"/>
+      <c r="DW3" s="67"/>
+      <c r="DX3" s="67"/>
+      <c r="DY3" s="67"/>
+      <c r="DZ3" s="67"/>
+      <c r="EA3" s="67"/>
+      <c r="EB3" s="67"/>
+      <c r="EC3" s="67"/>
+      <c r="ED3" s="67"/>
+      <c r="EE3" s="67"/>
+      <c r="EF3" s="67"/>
+      <c r="EG3" s="67"/>
+      <c r="EH3" s="67"/>
+      <c r="EI3" s="67"/>
+    </row>
+    <row r="4" spans="1:139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="14">
         <v>1</v>
       </c>
@@ -2095,7 +2091,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>41</v>
       </c>
@@ -2121,7 +2117,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>41</v>
       </c>
@@ -2148,7 +2144,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>41</v>
       </c>
@@ -2174,7 +2170,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>41</v>
       </c>
@@ -2200,7 +2196,7 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>41</v>
       </c>
@@ -2226,7 +2222,7 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>41</v>
       </c>
@@ -2252,7 +2248,7 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>41</v>
       </c>
@@ -2278,7 +2274,7 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>41</v>
       </c>
@@ -2304,36 +2300,38 @@
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:139" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:139" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="68" t="s">
-        <v>43</v>
+      <c r="B13" s="45" t="s">
+        <v>46</v>
       </c>
       <c r="C13" s="18">
         <v>22</v>
       </c>
       <c r="D13" s="18">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E13" s="32">
         <v>31</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="19">
+        <v>25</v>
+      </c>
       <c r="G13" s="20">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H13" s="21"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="18">
         <v>34</v>
@@ -2352,49 +2350,59 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="18">
         <v>38</v>
       </c>
       <c r="D15" s="18">
-        <v>6</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+        <v>12</v>
+      </c>
+      <c r="E15" s="19">
+        <v>41</v>
+      </c>
+      <c r="F15" s="19">
+        <v>9</v>
+      </c>
       <c r="G15" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="21"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="18">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D16" s="69">
         <v>5</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="4"/>
+      <c r="E16" s="19">
+        <v>52</v>
+      </c>
+      <c r="F16" s="19">
+        <v>3</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
       <c r="H16" s="17"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
     </row>
-    <row r="17" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>41</v>
       </c>
@@ -2402,7 +2410,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="18">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D17" s="18">
         <v>15</v>
@@ -2416,7 +2424,7 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
     </row>
-    <row r="18" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>41</v>
       </c>
@@ -2438,7 +2446,7 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
     </row>
-    <row r="19" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>41</v>
       </c>
@@ -2446,7 +2454,7 @@
         <v>33</v>
       </c>
       <c r="C19" s="18">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D19" s="18">
         <v>15</v>
@@ -2460,7 +2468,7 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
     </row>
-    <row r="20" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>41</v>
       </c>
@@ -2468,12 +2476,14 @@
         <v>37</v>
       </c>
       <c r="C20" s="18">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D20" s="18">
         <v>100</v>
       </c>
-      <c r="E20" s="19"/>
+      <c r="E20" s="19">
+        <v>38</v>
+      </c>
       <c r="F20" s="19"/>
       <c r="G20" s="4">
         <v>0</v>
@@ -2482,7 +2492,7 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>41</v>
       </c>
@@ -2504,7 +2514,7 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>41</v>
       </c>
@@ -2655,7 +2665,7 @@
       <c r="EH22" s="42"/>
       <c r="EI22" s="42"/>
     </row>
-    <row r="23" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
@@ -2683,7 +2693,7 @@
       <c r="Z23"/>
       <c r="AA23"/>
     </row>
-    <row r="24" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
@@ -2711,7 +2721,7 @@
       <c r="Z24"/>
       <c r="AA24"/>
     </row>
-    <row r="25" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:139" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -2739,7 +2749,7 @@
       <c r="Z25"/>
       <c r="AA25"/>
     </row>
-    <row r="26" spans="1:139" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:139" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -2767,7 +2777,7 @@
       <c r="Z26"/>
       <c r="AA26"/>
     </row>
-    <row r="27" spans="1:139" ht="36.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:139" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -2795,7 +2805,7 @@
       <c r="Z27"/>
       <c r="AA27"/>
     </row>
-    <row r="28" spans="1:139" ht="36.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:139" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -2823,7 +2833,7 @@
       <c r="Z28"/>
       <c r="AA28"/>
     </row>
-    <row r="29" spans="1:139" ht="36.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:139" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -2851,7 +2861,7 @@
       <c r="Z29"/>
       <c r="AA29"/>
     </row>
-    <row r="30" spans="1:139" ht="36.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:139" ht="36.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -2879,7 +2889,7 @@
       <c r="Z30"/>
       <c r="AA30"/>
     </row>
-    <row r="31" spans="1:139" ht="36.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:139" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
@@ -2907,7 +2917,7 @@
       <c r="Z31"/>
       <c r="AA31"/>
     </row>
-    <row r="32" spans="1:139" ht="36.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:139" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
@@ -2935,20 +2945,20 @@
       <c r="Z32"/>
       <c r="AA32"/>
     </row>
-    <row r="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -2976,7 +2986,7 @@
       <c r="Z49"/>
       <c r="AA49"/>
     </row>
-    <row r="50" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -3004,7 +3014,7 @@
       <c r="Z50"/>
       <c r="AA50"/>
     </row>
-    <row r="51" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -3032,7 +3042,7 @@
       <c r="Z51"/>
       <c r="AA51"/>
     </row>
-    <row r="52" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
@@ -3060,7 +3070,7 @@
       <c r="Z52"/>
       <c r="AA52"/>
     </row>
-    <row r="53" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
@@ -3088,7 +3098,7 @@
       <c r="Z53"/>
       <c r="AA53"/>
     </row>
-    <row r="54" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
@@ -3116,7 +3126,7 @@
       <c r="Z54"/>
       <c r="AA54"/>
     </row>
-    <row r="55" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
@@ -3144,7 +3154,7 @@
       <c r="Z55"/>
       <c r="AA55"/>
     </row>
-    <row r="56" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
@@ -3172,7 +3182,7 @@
       <c r="Z56"/>
       <c r="AA56"/>
     </row>
-    <row r="57" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
@@ -3200,7 +3210,7 @@
       <c r="Z57"/>
       <c r="AA57"/>
     </row>
-    <row r="58" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
@@ -3228,7 +3238,7 @@
       <c r="Z58"/>
       <c r="AA58"/>
     </row>
-    <row r="59" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
@@ -3256,7 +3266,7 @@
       <c r="Z59"/>
       <c r="AA59"/>
     </row>
-    <row r="60" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
@@ -3284,7 +3294,7 @@
       <c r="Z60"/>
       <c r="AA60"/>
     </row>
-    <row r="61" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
@@ -3312,7 +3322,7 @@
       <c r="Z61"/>
       <c r="AA61"/>
     </row>
-    <row r="62" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J62"/>
       <c r="K62"/>
       <c r="L62"/>
@@ -3332,7 +3342,7 @@
       <c r="Z62"/>
       <c r="AA62"/>
     </row>
-    <row r="63" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J63"/>
       <c r="K63"/>
       <c r="L63"/>
@@ -3352,7 +3362,7 @@
       <c r="Z63"/>
       <c r="AA63"/>
     </row>
-    <row r="64" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J64"/>
       <c r="K64"/>
       <c r="L64"/>
@@ -3372,7 +3382,7 @@
       <c r="Z64"/>
       <c r="AA64"/>
     </row>
-    <row r="65" spans="10:27" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="10:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J65"/>
       <c r="K65"/>
       <c r="L65"/>
@@ -3392,7 +3402,7 @@
       <c r="Z65"/>
       <c r="AA65"/>
     </row>
-    <row r="66" spans="10:27" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="10:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J66"/>
       <c r="K66"/>
       <c r="L66"/>
@@ -3414,21 +3424,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="CT3:CZ3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="DO3:EI3"/>
     <mergeCell ref="DA3:DG3"/>
     <mergeCell ref="DH3:DN3"/>
@@ -3445,6 +3440,21 @@
     <mergeCell ref="BY3:CE3"/>
     <mergeCell ref="CF3:CL3"/>
     <mergeCell ref="CM3:CS3"/>
+    <mergeCell ref="CT3:CZ3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:M22">
     <cfRule type="expression" dxfId="17" priority="10">
@@ -3530,7 +3540,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.51181102362204722" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="25" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="24" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
     <firstHeader xml:space="preserve">&amp;LSom note så tælles dagene ud fra projektstart- altså første dag vi blev tildelt grupper og projektet gik i gang.

</xml_diff>